<commit_message>
Add automatic table generation
</commit_message>
<xml_diff>
--- a/aaanalysis/data/benchmarks/INFO_benchmarks.xlsx
+++ b/aaanalysis/data/benchmarks/INFO_benchmarks.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Publication</t>
+    <t xml:space="preserve">Reference</t>
   </si>
   <si>
     <t xml:space="preserve">Label</t>
@@ -293,13 +293,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -322,10 +326,10 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -360,383 +364,383 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>185605</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="2" t="n">
         <v>705</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="n">
         <v>184900</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>59003</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="2" t="n">
         <v>163</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="2" t="n">
         <v>58840</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="2" t="n">
         <v>342</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="2" t="n">
         <v>118248</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="2" t="n">
         <v>35469</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="2" t="n">
         <v>82779</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="2" t="n">
         <v>573</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="2" t="n">
         <v>312976</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="2" t="n">
         <v>2416</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="2" t="n">
         <v>310560</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="2" t="n">
         <v>55001</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="2" t="n">
         <v>6492</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="2" t="n">
         <v>48509</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="2" t="n">
         <v>185605</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="2" t="n">
         <v>101082</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="2" t="n">
         <v>84523</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="2" t="n">
         <v>1414</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="2" t="n">
         <v>8484</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="2" t="n">
         <v>511</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="2" t="n">
         <v>903</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="2" t="n">
         <v>7935</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="2" t="n">
         <v>3364680</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="2" t="n">
         <v>3864</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="2" t="n">
         <v>4071</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="2" t="n">
         <v>2547</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="2" t="n">
         <v>614470</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="2" t="n">
         <v>897</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="2" t="n">
         <v>1650</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="2" t="n">
         <v>1835</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="2" t="n">
         <v>732398</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="2" t="n">
         <v>1045</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="2" t="n">
         <v>790</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="J11" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="2" t="n">
         <v>17408</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="2" t="n">
         <v>4432269</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="2" t="n">
         <v>8704</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="2" t="n">
         <v>8704</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="2" t="n">
         <v>6668</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="2" t="n">
         <v>2671690</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="2" t="n">
         <v>2574</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="2" t="n">
         <v>4094</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="2" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>